<commit_message>
VD/VA current limits added Col to col threshold limits addad
</commit_message>
<xml_diff>
--- a/colortable.xlsx
+++ b/colortable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="13650" yWindow="90" windowWidth="14805" windowHeight="13545"/>
   </bookViews>
   <sheets>
     <sheet name="ColorTable" sheetId="1" r:id="rId1"/>
@@ -261,12 +261,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFBFFF40"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -285,12 +279,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0066"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF004C00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -309,18 +297,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFBFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB2FFB2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF008080"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -339,12 +315,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00BFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF80BFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -412,6 +382,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF80FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD700"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0FFDD0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CAA4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8989"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC1C1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -564,13 +564,8 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -604,12 +599,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFC1C1"/>
+      <color rgb="FFFF8989"/>
+      <color rgb="FF00CAA4"/>
+      <color rgb="FF02CAA4"/>
+      <color rgb="FF0FFDD0"/>
+      <color rgb="FFFE6F48"/>
+      <color rgb="FFFF4B47"/>
+      <color rgb="FFFF6699"/>
+      <color rgb="FFFFD700"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -908,8 +921,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B3:Q31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,44 +941,44 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="43" t="s">
+      <c r="C3" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="44"/>
-      <c r="G3" s="42" t="s">
+      <c r="F3" s="39"/>
+      <c r="G3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="43"/>
-      <c r="I3" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" s="46" t="s">
+      <c r="H3" s="38"/>
+      <c r="I3" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="49" t="s">
+      <c r="M3" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="49" t="s">
+      <c r="N3" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="42" t="s">
+      <c r="O3" s="37" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="50">
+      <c r="B4" s="45">
         <v>0</v>
       </c>
       <c r="C4" s="4">
@@ -974,13 +987,13 @@
       <c r="D4" s="4">
         <v>0</v>
       </c>
-      <c r="E4" s="38">
-        <v>0</v>
-      </c>
-      <c r="F4" s="36"/>
+      <c r="E4" s="33">
+        <v>0</v>
+      </c>
+      <c r="F4" s="31"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="40">
+      <c r="H4" s="33"/>
+      <c r="I4" s="35">
         <f>C4/255</f>
         <v>0</v>
       </c>
@@ -992,8 +1005,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47">
+      <c r="M4" s="42"/>
+      <c r="N4" s="42">
         <v>2</v>
       </c>
       <c r="O4" s="4"/>
@@ -1002,7 +1015,7 @@
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="50">
+      <c r="B5" s="45">
         <v>1</v>
       </c>
       <c r="C5" s="4">
@@ -1011,13 +1024,13 @@
       <c r="D5" s="4">
         <v>127.5</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="33">
         <v>127.5</v>
       </c>
-      <c r="F5" s="36"/>
+      <c r="F5" s="31"/>
       <c r="G5" s="7"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="40">
+      <c r="H5" s="33"/>
+      <c r="I5" s="35">
         <f t="shared" ref="I5:I31" si="1">C5/255</f>
         <v>0.5</v>
       </c>
@@ -1029,8 +1042,8 @@
         <f t="shared" ref="K5:K31" si="3">E5/255</f>
         <v>0.5</v>
       </c>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47">
+      <c r="M5" s="42"/>
+      <c r="N5" s="42">
         <v>3</v>
       </c>
       <c r="O5" s="4"/>
@@ -1039,42 +1052,44 @@
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="50">
+      <c r="B6" s="45">
         <v>2</v>
       </c>
       <c r="C6" s="4">
-        <v>191.25</v>
+        <v>255</v>
       </c>
       <c r="D6" s="4">
-        <v>255</v>
-      </c>
-      <c r="E6" s="38">
-        <v>63.75</v>
-      </c>
-      <c r="F6" s="36"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="40">
-        <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>193</v>
+      </c>
+      <c r="E6" s="33">
+        <v>193</v>
+      </c>
+      <c r="F6" s="31"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="35">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="J6" s="6">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.75686274509803919</v>
       </c>
       <c r="K6" s="6">
         <f t="shared" si="3"/>
-        <v>0.25</v>
-      </c>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
+        <v>0.75686274509803919</v>
+      </c>
+      <c r="M6" s="42"/>
+      <c r="N6" s="42">
+        <v>15</v>
+      </c>
       <c r="O6" s="4"/>
       <c r="Q6" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="50">
+      <c r="B7" s="45">
         <v>3</v>
       </c>
       <c r="C7" s="4">
@@ -1083,13 +1098,13 @@
       <c r="D7" s="4">
         <v>255</v>
       </c>
-      <c r="E7" s="38">
-        <v>255</v>
-      </c>
-      <c r="F7" s="36"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="40">
+      <c r="E7" s="33">
+        <v>255</v>
+      </c>
+      <c r="F7" s="31"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1101,15 +1116,15 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M7" s="47"/>
-      <c r="N7" s="47"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="42"/>
       <c r="O7" s="4"/>
       <c r="Q7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="50">
+      <c r="B8" s="45">
         <v>4</v>
       </c>
       <c r="C8" s="4">
@@ -1118,13 +1133,13 @@
       <c r="D8" s="4">
         <v>0</v>
       </c>
-      <c r="E8" s="38">
-        <v>0</v>
-      </c>
-      <c r="F8" s="36"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="40">
+      <c r="E8" s="33">
+        <v>0</v>
+      </c>
+      <c r="F8" s="31"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="35">
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
@@ -1136,8 +1151,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47">
+      <c r="M8" s="42"/>
+      <c r="N8" s="42">
         <v>1</v>
       </c>
       <c r="O8" s="4"/>
@@ -1146,7 +1161,7 @@
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="50">
+      <c r="B9" s="45">
         <v>5</v>
       </c>
       <c r="C9" s="4">
@@ -1155,13 +1170,13 @@
       <c r="D9" s="4">
         <v>0</v>
       </c>
-      <c r="E9" s="38">
-        <v>0</v>
-      </c>
-      <c r="F9" s="36"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="40">
+      <c r="E9" s="33">
+        <v>0</v>
+      </c>
+      <c r="F9" s="31"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1173,10 +1188,10 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M9" s="47">
-        <v>1</v>
-      </c>
-      <c r="N9" s="47">
+      <c r="M9" s="42">
+        <v>1</v>
+      </c>
+      <c r="N9" s="42">
         <v>0</v>
       </c>
       <c r="O9" s="4">
@@ -1187,42 +1202,44 @@
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="50">
+      <c r="B10" s="45">
         <v>6</v>
       </c>
       <c r="C10" s="4">
-        <v>255</v>
+        <v>15</v>
       </c>
       <c r="D10" s="4">
-        <v>0</v>
-      </c>
-      <c r="E10" s="38">
-        <v>102</v>
-      </c>
-      <c r="F10" s="36"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="40">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>253</v>
+      </c>
+      <c r="E10" s="33">
+        <v>208</v>
+      </c>
+      <c r="F10" s="31"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="35">
+        <f t="shared" si="1"/>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="J10" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.99215686274509807</v>
       </c>
       <c r="K10" s="6">
         <f t="shared" si="3"/>
-        <v>0.4</v>
-      </c>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
+        <v>0.81568627450980391</v>
+      </c>
+      <c r="M10" s="42"/>
+      <c r="N10" s="42">
+        <v>19</v>
+      </c>
       <c r="O10" s="4"/>
       <c r="Q10" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="50">
+      <c r="B11" s="45">
         <v>7</v>
       </c>
       <c r="C11" s="4">
@@ -1231,13 +1248,13 @@
       <c r="D11" s="4">
         <v>76.5</v>
       </c>
-      <c r="E11" s="38">
-        <v>0</v>
-      </c>
-      <c r="F11" s="36"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="40">
+      <c r="E11" s="33">
+        <v>0</v>
+      </c>
+      <c r="F11" s="31"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1249,15 +1266,15 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M11" s="47"/>
-      <c r="N11" s="47"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="42"/>
       <c r="O11" s="4"/>
       <c r="Q11" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="50">
+      <c r="B12" s="45">
         <v>8</v>
       </c>
       <c r="C12" s="4">
@@ -1266,13 +1283,13 @@
       <c r="D12" s="4">
         <v>191.25</v>
       </c>
-      <c r="E12" s="38">
-        <v>0</v>
-      </c>
-      <c r="F12" s="36"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="40">
+      <c r="E12" s="33">
+        <v>0</v>
+      </c>
+      <c r="F12" s="31"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1284,10 +1301,10 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M12" s="47">
-        <v>0</v>
-      </c>
-      <c r="N12" s="47">
+      <c r="M12" s="42">
+        <v>0</v>
+      </c>
+      <c r="N12" s="42">
         <v>23</v>
       </c>
       <c r="O12" s="4">
@@ -1298,7 +1315,7 @@
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="50">
+      <c r="B13" s="45">
         <v>9</v>
       </c>
       <c r="C13" s="4">
@@ -1307,13 +1324,13 @@
       <c r="D13" s="4">
         <v>255</v>
       </c>
-      <c r="E13" s="38">
-        <v>0</v>
-      </c>
-      <c r="F13" s="36"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="40">
+      <c r="E13" s="33">
+        <v>0</v>
+      </c>
+      <c r="F13" s="31"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1325,85 +1342,89 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M13" s="47"/>
-      <c r="N13" s="47"/>
+      <c r="M13" s="42"/>
+      <c r="N13" s="42"/>
       <c r="O13" s="4"/>
       <c r="Q13" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="50">
+      <c r="B14" s="45">
         <v>10</v>
       </c>
       <c r="C14" s="4">
-        <v>191.25</v>
+        <v>0</v>
       </c>
       <c r="D14" s="4">
-        <v>255</v>
-      </c>
-      <c r="E14" s="38">
-        <v>0</v>
-      </c>
-      <c r="F14" s="36"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="40">
-        <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>202</v>
+      </c>
+      <c r="E14" s="33">
+        <v>164</v>
+      </c>
+      <c r="F14" s="31"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="J14" s="6">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.792156862745098</v>
       </c>
       <c r="K14" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M14" s="47"/>
-      <c r="N14" s="47"/>
+        <v>0.64313725490196083</v>
+      </c>
+      <c r="M14" s="42"/>
+      <c r="N14" s="42">
+        <v>18</v>
+      </c>
       <c r="O14" s="4"/>
       <c r="Q14" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="50">
+      <c r="B15" s="45">
         <v>11</v>
       </c>
       <c r="C15" s="4">
-        <v>178.5</v>
+        <v>255</v>
       </c>
       <c r="D15" s="4">
-        <v>255</v>
-      </c>
-      <c r="E15" s="38">
-        <v>178.5</v>
-      </c>
-      <c r="F15" s="36"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="40">
-        <f t="shared" si="1"/>
-        <v>0.7</v>
+        <v>215</v>
+      </c>
+      <c r="E15" s="33">
+        <v>0</v>
+      </c>
+      <c r="F15" s="31"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="35">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="J15" s="6">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.84313725490196079</v>
       </c>
       <c r="K15" s="6">
         <f t="shared" si="3"/>
-        <v>0.7</v>
-      </c>
-      <c r="M15" s="47"/>
-      <c r="N15" s="47"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="42"/>
+      <c r="N15" s="42">
+        <v>16</v>
+      </c>
       <c r="O15" s="4"/>
       <c r="Q15" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="50">
+      <c r="B16" s="45">
         <v>12</v>
       </c>
       <c r="C16" s="4">
@@ -1412,13 +1433,13 @@
       <c r="D16" s="4">
         <v>127.5</v>
       </c>
-      <c r="E16" s="38">
+      <c r="E16" s="33">
         <v>127.5</v>
       </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="40">
+      <c r="F16" s="31"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1430,17 +1451,17 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="M16" s="47">
+      <c r="M16" s="42">
         <v>8</v>
       </c>
-      <c r="N16" s="47"/>
+      <c r="N16" s="42"/>
       <c r="O16" s="4"/>
       <c r="Q16" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="50">
+      <c r="B17" s="45">
         <v>13</v>
       </c>
       <c r="C17" s="4">
@@ -1449,13 +1470,13 @@
       <c r="D17" s="4">
         <v>0</v>
       </c>
-      <c r="E17" s="38">
-        <v>255</v>
-      </c>
-      <c r="F17" s="36"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="40">
+      <c r="E17" s="33">
+        <v>255</v>
+      </c>
+      <c r="F17" s="31"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1467,10 +1488,10 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M17" s="47">
+      <c r="M17" s="42">
         <v>9</v>
       </c>
-      <c r="N17" s="47">
+      <c r="N17" s="42">
         <v>22</v>
       </c>
       <c r="O17" s="4">
@@ -1481,7 +1502,7 @@
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="50">
+      <c r="B18" s="45">
         <v>14</v>
       </c>
       <c r="C18" s="4">
@@ -1490,13 +1511,13 @@
       <c r="D18" s="4">
         <v>127.5</v>
       </c>
-      <c r="E18" s="38">
-        <v>255</v>
-      </c>
-      <c r="F18" s="36"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="40">
+      <c r="E18" s="33">
+        <v>255</v>
+      </c>
+      <c r="F18" s="31"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="35">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
@@ -1508,52 +1529,56 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M18" s="47">
+      <c r="M18" s="42">
         <v>10</v>
       </c>
-      <c r="N18" s="47"/>
+      <c r="N18" s="42">
+        <v>21</v>
+      </c>
       <c r="O18" s="4"/>
       <c r="Q18" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="50">
+      <c r="B19" s="45">
         <v>15</v>
       </c>
       <c r="C19" s="4">
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="D19" s="4">
-        <v>191.25</v>
-      </c>
-      <c r="E19" s="38">
-        <v>255</v>
-      </c>
-      <c r="F19" s="36"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="40">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>137</v>
+      </c>
+      <c r="E19" s="33">
+        <v>137</v>
+      </c>
+      <c r="F19" s="31"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="35">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="J19" s="6">
         <f t="shared" si="2"/>
-        <v>0.75</v>
+        <v>0.53725490196078429</v>
       </c>
       <c r="K19" s="6">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="M19" s="47"/>
-      <c r="N19" s="47"/>
+        <v>0.53725490196078429</v>
+      </c>
+      <c r="M19" s="42"/>
+      <c r="N19" s="42">
+        <v>14</v>
+      </c>
       <c r="O19" s="4"/>
       <c r="Q19" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B20" s="50">
+      <c r="B20" s="45">
         <v>16</v>
       </c>
       <c r="C20" s="4">
@@ -1562,13 +1587,13 @@
       <c r="D20" s="4">
         <v>191.25</v>
       </c>
-      <c r="E20" s="38">
-        <v>255</v>
-      </c>
-      <c r="F20" s="36"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="40">
+      <c r="E20" s="33">
+        <v>255</v>
+      </c>
+      <c r="F20" s="31"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="35">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -1580,17 +1605,19 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M20" s="47">
+      <c r="M20" s="42">
         <v>11</v>
       </c>
-      <c r="N20" s="47"/>
+      <c r="N20" s="42">
+        <v>20</v>
+      </c>
       <c r="O20" s="4"/>
       <c r="Q20" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B21" s="50">
+      <c r="B21" s="45">
         <v>17</v>
       </c>
       <c r="C21" s="4">
@@ -1599,13 +1626,13 @@
       <c r="D21" s="4">
         <v>255</v>
       </c>
-      <c r="E21" s="38">
-        <v>255</v>
-      </c>
-      <c r="F21" s="36"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="40">
+      <c r="E21" s="33">
+        <v>255</v>
+      </c>
+      <c r="F21" s="31"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1617,8 +1644,8 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M21" s="47"/>
-      <c r="N21" s="47">
+      <c r="M21" s="42"/>
+      <c r="N21" s="42">
         <v>8</v>
       </c>
       <c r="O21" s="4"/>
@@ -1627,7 +1654,7 @@
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B22" s="50">
+      <c r="B22" s="45">
         <v>18</v>
       </c>
       <c r="C22" s="4">
@@ -1636,13 +1663,13 @@
       <c r="D22" s="4">
         <v>255</v>
       </c>
-      <c r="E22" s="38">
-        <v>255</v>
-      </c>
-      <c r="F22" s="36"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="40">
+      <c r="E22" s="33">
+        <v>255</v>
+      </c>
+      <c r="F22" s="31"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="35">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -1654,17 +1681,17 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M22" s="47">
+      <c r="M22" s="42">
         <v>12</v>
       </c>
-      <c r="N22" s="47"/>
+      <c r="N22" s="42"/>
       <c r="O22" s="4"/>
       <c r="Q22" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B23" s="50">
+      <c r="B23" s="45">
         <v>19</v>
       </c>
       <c r="C23" s="4">
@@ -1673,13 +1700,13 @@
       <c r="D23" s="4">
         <v>63.75</v>
       </c>
-      <c r="E23" s="38">
-        <v>0</v>
-      </c>
-      <c r="F23" s="36"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="40">
+      <c r="E23" s="33">
+        <v>0</v>
+      </c>
+      <c r="F23" s="31"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="35">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -1691,8 +1718,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M23" s="47"/>
-      <c r="N23" s="47">
+      <c r="M23" s="42"/>
+      <c r="N23" s="42">
         <v>11</v>
       </c>
       <c r="O23" s="4"/>
@@ -1701,7 +1728,7 @@
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="50">
+      <c r="B24" s="45">
         <v>20</v>
       </c>
       <c r="C24" s="4">
@@ -1710,13 +1737,13 @@
       <c r="D24" s="4">
         <v>127.5</v>
       </c>
-      <c r="E24" s="38">
-        <v>0</v>
-      </c>
-      <c r="F24" s="36"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="40">
+      <c r="E24" s="33">
+        <v>0</v>
+      </c>
+      <c r="F24" s="31"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="35">
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
@@ -1728,8 +1755,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M24" s="47"/>
-      <c r="N24" s="47">
+      <c r="M24" s="42"/>
+      <c r="N24" s="42">
         <v>12</v>
       </c>
       <c r="O24" s="4"/>
@@ -1738,7 +1765,7 @@
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" s="50">
+      <c r="B25" s="45">
         <v>21</v>
       </c>
       <c r="C25" s="4">
@@ -1747,13 +1774,13 @@
       <c r="D25" s="4">
         <v>127.5</v>
       </c>
-      <c r="E25" s="38">
+      <c r="E25" s="33">
         <v>63.75</v>
       </c>
-      <c r="F25" s="36"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="40">
+      <c r="F25" s="31"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1765,17 +1792,17 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="M25" s="47">
+      <c r="M25" s="42">
         <v>3</v>
       </c>
-      <c r="N25" s="47"/>
+      <c r="N25" s="42"/>
       <c r="O25" s="4"/>
       <c r="Q25" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="50">
+      <c r="B26" s="45">
         <v>22</v>
       </c>
       <c r="C26" s="4">
@@ -1784,13 +1811,13 @@
       <c r="D26" s="4">
         <v>127.5</v>
       </c>
-      <c r="E26" s="38">
-        <v>0</v>
-      </c>
-      <c r="F26" s="36"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="40">
+      <c r="E26" s="33">
+        <v>0</v>
+      </c>
+      <c r="F26" s="31"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1802,15 +1829,15 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M26" s="47"/>
-      <c r="N26" s="47">
+      <c r="M26" s="42"/>
+      <c r="N26" s="42">
         <v>7</v>
       </c>
       <c r="O26" s="4"/>
       <c r="Q26" s="3"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B27" s="50">
+      <c r="B27" s="45">
         <v>23</v>
       </c>
       <c r="C27" s="4">
@@ -1819,13 +1846,13 @@
       <c r="D27" s="4">
         <v>255</v>
       </c>
-      <c r="E27" s="38">
-        <v>0</v>
-      </c>
-      <c r="F27" s="36"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="40">
+      <c r="E27" s="33">
+        <v>0</v>
+      </c>
+      <c r="F27" s="31"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1837,10 +1864,10 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M27" s="47">
+      <c r="M27" s="42">
         <v>2</v>
       </c>
-      <c r="N27" s="47">
+      <c r="N27" s="42">
         <v>6</v>
       </c>
       <c r="O27" s="4">
@@ -1851,7 +1878,7 @@
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B28" s="50">
+      <c r="B28" s="45">
         <v>24</v>
       </c>
       <c r="C28" s="4">
@@ -1860,13 +1887,13 @@
       <c r="D28" s="4">
         <v>255</v>
       </c>
-      <c r="E28" s="38">
+      <c r="E28" s="33">
         <v>216.75</v>
       </c>
-      <c r="F28" s="36"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="40">
+      <c r="F28" s="31"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1878,10 +1905,10 @@
         <f t="shared" si="3"/>
         <v>0.85</v>
       </c>
-      <c r="M28" s="47">
+      <c r="M28" s="42">
         <v>4</v>
       </c>
-      <c r="N28" s="47">
+      <c r="N28" s="42">
         <v>4</v>
       </c>
       <c r="O28" s="4"/>
@@ -1890,7 +1917,7 @@
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B29" s="50">
+      <c r="B29" s="45">
         <v>25</v>
       </c>
       <c r="C29" s="4">
@@ -1899,13 +1926,13 @@
       <c r="D29" s="4">
         <v>0</v>
       </c>
-      <c r="E29" s="38">
+      <c r="E29" s="33">
         <v>127.5</v>
       </c>
-      <c r="F29" s="36"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="40">
+      <c r="F29" s="31"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="35">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -1917,10 +1944,10 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="M29" s="47">
+      <c r="M29" s="42">
         <v>5</v>
       </c>
-      <c r="N29" s="47">
+      <c r="N29" s="42">
         <v>13</v>
       </c>
       <c r="O29" s="4">
@@ -1931,7 +1958,7 @@
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B30" s="50">
+      <c r="B30" s="45">
         <v>26</v>
       </c>
       <c r="C30" s="4">
@@ -1940,13 +1967,13 @@
       <c r="D30" s="4">
         <v>0</v>
       </c>
-      <c r="E30" s="38">
-        <v>255</v>
-      </c>
-      <c r="F30" s="36"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="40">
+      <c r="E30" s="33">
+        <v>255</v>
+      </c>
+      <c r="F30" s="31"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1958,10 +1985,10 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M30" s="47">
+      <c r="M30" s="42">
         <v>6</v>
       </c>
-      <c r="N30" s="47">
+      <c r="N30" s="42">
         <v>9</v>
       </c>
       <c r="O30" s="4"/>
@@ -1970,40 +1997,40 @@
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="51">
+      <c r="B31" s="46">
         <v>27</v>
       </c>
-      <c r="C31" s="33">
-        <v>255</v>
-      </c>
-      <c r="D31" s="33">
+      <c r="C31" s="28">
+        <v>255</v>
+      </c>
+      <c r="D31" s="28">
         <v>127.5</v>
       </c>
-      <c r="E31" s="39">
-        <v>255</v>
-      </c>
-      <c r="F31" s="37"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="41">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J31" s="35">
+      <c r="E31" s="34">
+        <v>255</v>
+      </c>
+      <c r="F31" s="32"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="36">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J31" s="30">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="K31" s="35">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="M31" s="48">
+      <c r="K31" s="30">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="M31" s="43">
         <v>7</v>
       </c>
-      <c r="N31" s="48">
+      <c r="N31" s="43">
         <v>10</v>
       </c>
-      <c r="O31" s="33"/>
+      <c r="O31" s="28"/>
       <c r="Q31" s="3" t="s">
         <v>27</v>
       </c>
@@ -2020,7 +2047,7 @@
   <dimension ref="A3:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B15"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2142,7 +2169,7 @@
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A2:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
changes in colors code
to have uniformity between class and fail color code.
</commit_message>
<xml_diff>
--- a/colortable.xlsx
+++ b/colortable.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="180" windowWidth="14955" windowHeight="13545"/>
+    <workbookView xWindow="180" yWindow="180" windowWidth="14955" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="ColorTable" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ColorTable!$B$3:$M$41</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>R</t>
   </si>
@@ -42,15 +42,18 @@
   <si>
     <t>Bin</t>
   </si>
+  <si>
+    <t>5 not used</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,12 +236,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF787828"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFB46400"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -257,19 +254,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDCFF3C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA0B41E"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF78FF28"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF665C20"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9C9C20"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -447,8 +450,8 @@
     <xf numFmtId="0" fontId="0" fillId="26" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -463,7 +466,7 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -495,20 +498,22 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="31" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FF9C9C20"/>
+      <color rgb="FF665C20"/>
       <color rgb="FFB3FF85"/>
       <color rgb="FF79FF79"/>
       <color rgb="FFFBA06D"/>
@@ -517,8 +522,6 @@
       <color rgb="FFD91D1D"/>
       <color rgb="FFFFC1C1"/>
       <color rgb="FFFF8989"/>
-      <color rgb="FF00CAA4"/>
-      <color rgb="FF02CAA4"/>
     </mruColors>
   </colors>
   <extLst>
@@ -530,9 +533,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -570,7 +573,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -604,7 +607,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -639,10 +641,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -815,17 +816,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Tabelle1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:N45"/>
+  <dimension ref="A2:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.28515625" customWidth="1"/>
     <col min="3" max="5" width="4.7109375" customWidth="1"/>
@@ -835,10 +836,10 @@
     <col min="12" max="14" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" s="43"/>
     </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="1" customFormat="1">
       <c r="A3" s="44"/>
       <c r="B3" s="54" t="s">
         <v>3</v>
@@ -875,7 +876,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" s="43"/>
       <c r="B4" s="14">
         <v>0</v>
@@ -907,7 +908,7 @@
       <c r="M4" s="15"/>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="43"/>
       <c r="B5" s="12">
         <v>1</v>
@@ -941,7 +942,7 @@
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" s="43"/>
       <c r="B6" s="12">
         <v>2</v>
@@ -975,7 +976,7 @@
       </c>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" s="43"/>
       <c r="B7" s="13">
         <v>3</v>
@@ -1005,18 +1006,21 @@
       </c>
       <c r="L7" s="5"/>
       <c r="M7" s="5">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="N7" s="5"/>
-    </row>
-    <row r="8" spans="1:14" s="45" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="45" customFormat="1" ht="5.0999999999999996" customHeight="1">
       <c r="B8" s="47"/>
       <c r="G8" s="48"/>
       <c r="H8" s="49"/>
       <c r="I8" s="49"/>
       <c r="J8" s="49"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" s="43"/>
       <c r="B9" s="14">
         <v>4</v>
@@ -1050,7 +1054,7 @@
       </c>
       <c r="N9" s="15"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="43"/>
       <c r="B10" s="12">
         <v>5</v>
@@ -1088,7 +1092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" s="43"/>
       <c r="B11" s="12">
         <v>6</v>
@@ -1120,7 +1124,7 @@
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" s="43"/>
       <c r="B12" s="12">
         <v>7</v>
@@ -1154,7 +1158,7 @@
       </c>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" s="43"/>
       <c r="B13" s="12">
         <v>8</v>
@@ -1188,7 +1192,7 @@
       </c>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" s="43"/>
       <c r="B14" s="13">
         <v>9</v>
@@ -1224,14 +1228,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="45" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" s="45" customFormat="1" ht="5.0999999999999996" customHeight="1">
       <c r="B15" s="47"/>
       <c r="G15" s="48"/>
       <c r="H15" s="49"/>
       <c r="I15" s="49"/>
       <c r="J15" s="49"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" s="43"/>
       <c r="B16" s="14">
         <v>10</v>
@@ -1260,12 +1264,12 @@
         <v>0</v>
       </c>
       <c r="L16" s="15"/>
-      <c r="M16" s="63">
-        <v>6</v>
+      <c r="M16" s="60">
+        <v>7</v>
       </c>
       <c r="N16" s="15"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14">
       <c r="A17" s="43"/>
       <c r="B17" s="12">
         <v>11</v>
@@ -1294,12 +1298,10 @@
         <v>0</v>
       </c>
       <c r="L17" s="3"/>
-      <c r="M17" s="64">
-        <v>7</v>
-      </c>
+      <c r="M17" s="61"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14">
       <c r="A18" s="43"/>
       <c r="B18" s="12">
         <v>12</v>
@@ -1331,7 +1333,7 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="A19" s="43"/>
       <c r="B19" s="13">
         <v>13</v>
@@ -1365,102 +1367,102 @@
       </c>
       <c r="N19" s="5"/>
     </row>
-    <row r="20" spans="1:14" s="45" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" s="45" customFormat="1" ht="5.0999999999999996" customHeight="1">
       <c r="B20" s="47"/>
       <c r="G20" s="48"/>
       <c r="H20" s="49"/>
       <c r="I20" s="49"/>
       <c r="J20" s="49"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14">
       <c r="A21" s="45"/>
       <c r="B21" s="14">
         <v>14</v>
       </c>
       <c r="C21" s="15">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="D21" s="15">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="E21" s="50">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F21" s="53"/>
-      <c r="G21" s="59"/>
+      <c r="G21" s="62"/>
       <c r="H21" s="57">
         <f t="shared" si="1"/>
-        <v>0.47058823529411764</v>
+        <v>0.4</v>
       </c>
       <c r="I21" s="57">
         <f t="shared" si="2"/>
-        <v>0.47058823529411764</v>
+        <v>0.36078431372549019</v>
       </c>
       <c r="J21" s="57">
         <f t="shared" si="3"/>
-        <v>0.15686274509803921</v>
+        <v>0.12549019607843137</v>
       </c>
       <c r="L21" s="15"/>
-      <c r="M21" s="63">
-        <v>14</v>
+      <c r="M21" s="60">
+        <v>9</v>
       </c>
       <c r="N21" s="15">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14">
       <c r="A22" s="43"/>
       <c r="B22" s="12">
         <v>15</v>
       </c>
       <c r="C22" s="3">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D22" s="3">
-        <v>180</v>
+        <v>156</v>
       </c>
       <c r="E22" s="9">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F22" s="7"/>
-      <c r="G22" s="61"/>
+      <c r="G22" s="63"/>
       <c r="H22" s="4">
         <f t="shared" si="1"/>
-        <v>0.62745098039215685</v>
+        <v>0.61176470588235299</v>
       </c>
       <c r="I22" s="4">
         <f t="shared" si="2"/>
-        <v>0.70588235294117652</v>
+        <v>0.61176470588235299</v>
       </c>
       <c r="J22" s="4">
         <f t="shared" si="3"/>
-        <v>0.11764705882352941</v>
+        <v>0.12549019607843137</v>
       </c>
       <c r="L22" s="3"/>
-      <c r="M22" s="64">
-        <v>15</v>
+      <c r="M22" s="61">
+        <v>10</v>
       </c>
       <c r="N22" s="3"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14">
       <c r="A23" s="43"/>
       <c r="B23" s="12">
         <v>16</v>
       </c>
       <c r="C23" s="3">
-        <v>220</v>
+        <v>255</v>
       </c>
       <c r="D23" s="3">
         <v>255</v>
       </c>
       <c r="E23" s="9">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="F23" s="7"/>
-      <c r="G23" s="60"/>
+      <c r="G23" s="64"/>
       <c r="H23" s="4">
         <f t="shared" si="1"/>
-        <v>0.86274509803921573</v>
+        <v>1</v>
       </c>
       <c r="I23" s="4">
         <f t="shared" si="2"/>
@@ -1468,19 +1470,19 @@
       </c>
       <c r="J23" s="4">
         <f t="shared" si="3"/>
-        <v>0.23529411764705882</v>
+        <v>0</v>
       </c>
       <c r="L23" s="3">
         <v>4</v>
       </c>
-      <c r="M23" s="64">
-        <v>16</v>
+      <c r="M23" s="61">
+        <v>6</v>
       </c>
       <c r="N23" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14">
       <c r="A24" s="43"/>
       <c r="B24" s="13">
         <v>17</v>
@@ -1510,20 +1512,20 @@
       </c>
       <c r="L24" s="5"/>
       <c r="M24" s="5">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="N24" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="45" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="45" customFormat="1" ht="5.0999999999999996" customHeight="1">
       <c r="B25" s="47"/>
       <c r="G25" s="48"/>
       <c r="H25" s="49"/>
       <c r="I25" s="49"/>
       <c r="J25" s="49"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14">
       <c r="A26" s="43"/>
       <c r="B26" s="14">
         <v>18</v>
@@ -1554,14 +1556,14 @@
       <c r="L26" s="15">
         <v>2</v>
       </c>
-      <c r="M26" s="63">
-        <v>17</v>
+      <c r="M26" s="60">
+        <v>22</v>
       </c>
       <c r="N26" s="15">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14">
       <c r="A27" s="46"/>
       <c r="B27" s="12">
         <v>19</v>
@@ -1595,7 +1597,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14">
       <c r="A28" s="46"/>
       <c r="B28" s="12">
         <v>20</v>
@@ -1631,7 +1633,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14">
       <c r="A29" s="46"/>
       <c r="B29" s="12">
         <v>21</v>
@@ -1663,7 +1665,7 @@
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14">
       <c r="A30" s="43"/>
       <c r="B30" s="13">
         <v>22</v>
@@ -1697,14 +1699,14 @@
       </c>
       <c r="N30" s="5"/>
     </row>
-    <row r="31" spans="1:14" s="45" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" s="45" customFormat="1" ht="5.0999999999999996" customHeight="1">
       <c r="B31" s="47"/>
       <c r="G31" s="48"/>
       <c r="H31" s="49"/>
       <c r="I31" s="49"/>
       <c r="J31" s="49"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14">
       <c r="A32" s="43"/>
       <c r="B32" s="14">
         <v>23</v>
@@ -1736,13 +1738,13 @@
         <v>3</v>
       </c>
       <c r="M32" s="15">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="N32" s="15">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14">
       <c r="A33" s="45"/>
       <c r="B33" s="12">
         <v>24</v>
@@ -1772,13 +1774,13 @@
       </c>
       <c r="L33" s="3"/>
       <c r="M33" s="3">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="N33" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14">
       <c r="A34" s="45"/>
       <c r="B34" s="12">
         <v>25</v>
@@ -1808,11 +1810,11 @@
       </c>
       <c r="L34" s="3"/>
       <c r="M34" s="3">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="N34" s="3"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14">
       <c r="A35" s="45"/>
       <c r="B35" s="13">
         <v>26</v>
@@ -1842,20 +1844,20 @@
       </c>
       <c r="L35" s="5"/>
       <c r="M35" s="5">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="N35" s="5">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:14" s="45" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" s="45" customFormat="1" ht="5.0999999999999996" customHeight="1">
       <c r="B36" s="47"/>
       <c r="G36" s="48"/>
       <c r="H36" s="49"/>
       <c r="I36" s="49"/>
       <c r="J36" s="49"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14">
       <c r="A37" s="45"/>
       <c r="B37" s="14">
         <v>27</v>
@@ -1887,7 +1889,7 @@
       <c r="M37" s="15"/>
       <c r="N37" s="15"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14">
       <c r="A38" s="45"/>
       <c r="B38" s="12">
         <v>28</v>
@@ -1925,7 +1927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14">
       <c r="A39" s="45"/>
       <c r="B39" s="12">
         <v>29</v>
@@ -1940,7 +1942,7 @@
         <v>40</v>
       </c>
       <c r="F39" s="7"/>
-      <c r="G39" s="62"/>
+      <c r="G39" s="59"/>
       <c r="H39" s="4">
         <f t="shared" si="1"/>
         <v>0.47058823529411764</v>
@@ -1957,7 +1959,7 @@
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14">
       <c r="A40" s="45"/>
       <c r="B40" s="12">
         <v>30</v>
@@ -1986,14 +1988,12 @@
         <v>0.50980392156862742</v>
       </c>
       <c r="L40" s="3"/>
-      <c r="M40" s="3">
-        <v>22</v>
-      </c>
+      <c r="M40" s="3"/>
       <c r="N40" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14">
       <c r="A41" s="43"/>
       <c r="B41" s="13">
         <v>31</v>
@@ -2022,19 +2022,21 @@
         <v>0.62745098039215685</v>
       </c>
       <c r="L41" s="5"/>
-      <c r="M41" s="5"/>
+      <c r="M41" s="5">
+        <v>17</v>
+      </c>
       <c r="N41" s="5"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14">
       <c r="A42" s="43"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14">
       <c r="A43" s="43"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14">
       <c r="A44" s="43"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14">
       <c r="A45" s="43"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to lastest official test version
</commit_message>
<xml_diff>
--- a/colortable.xlsx
+++ b/colortable.xlsx
@@ -822,8 +822,8 @@
   </sheetPr>
   <dimension ref="A2:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1330,7 +1330,9 @@
         <v>0</v>
       </c>
       <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
+      <c r="M18" s="3">
+        <v>8</v>
+      </c>
       <c r="N18" s="3"/>
     </row>
     <row r="19" spans="1:14">
@@ -1362,9 +1364,7 @@
         <v>0.39215686274509803</v>
       </c>
       <c r="L19" s="5"/>
-      <c r="M19" s="5">
-        <v>8</v>
-      </c>
+      <c r="M19" s="5"/>
       <c r="N19" s="5"/>
     </row>
     <row r="20" spans="1:14" s="45" customFormat="1" ht="5.0999999999999996" customHeight="1">

</xml_diff>